<commit_message>
nominal changes to test the app how a push affects the app while it running
</commit_message>
<xml_diff>
--- a/Testing Manager.xlsx
+++ b/Testing Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\2024-10-ATAA-Forge\scouting-xtreme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94F4219-E81A-4772-90C7-9ACB2FD693DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338D0104-E534-460B-AB7F-A2539226F104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" activeTab="3" xr2:uid="{02701ECD-E265-41D5-A2A7-3CC6CA32D865}"/>
+    <workbookView xWindow="12877" yWindow="0" windowWidth="13125" windowHeight="15563" activeTab="2" xr2:uid="{02701ECD-E265-41D5-A2A7-3CC6CA32D865}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Runs" sheetId="1" r:id="rId1"/>
@@ -353,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -374,37 +374,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="28">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF156082"/>
-          <bgColor rgb="FF156082"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -495,6 +470,30 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF156082"/>
+          <bgColor rgb="FF156082"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -800,8 +799,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>128592</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Test Suite Name">
@@ -824,7 +823,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -883,8 +882,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>123829</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="Test Case Name">
@@ -907,7 +906,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1008,7 +1007,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BE361D65-1673-4F44-9EE8-1F2B584CC1AE}" name="tbl_TestSuites" displayName="tbl_TestSuites" ref="A1:J6" totalsRowShown="0" headerRowDxfId="1" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BE361D65-1673-4F44-9EE8-1F2B584CC1AE}" name="tbl_TestSuites" displayName="tbl_TestSuites" ref="A1:J6" totalsRowShown="0" headerRowDxfId="16" dataCellStyle="Normal">
   <autoFilter ref="A1:J6" xr:uid="{BE361D65-1673-4F44-9EE8-1F2B584CC1AE}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{14E89959-557D-4658-8F3A-7444B6EEF92A}" name="Test Suite ID" dataCellStyle="Normal"/>
@@ -1037,34 +1036,34 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{013E8841-AA34-4C82-B9AA-E95138FF2B02}" name="tbl_TestCases" displayName="tbl_TestCases" ref="A17:M40" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{013E8841-AA34-4C82-B9AA-E95138FF2B02}" name="tbl_TestCases" displayName="tbl_TestCases" ref="A17:M40" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" dataCellStyle="Normal">
   <autoFilter ref="A17:M40" xr:uid="{013E8841-AA34-4C82-B9AA-E95138FF2B02}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{27574F06-5BA9-4E63-97C7-825783688D46}" name="Test Case ID" dataDxfId="14" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{B526EB36-9DB5-49C2-8DA1-334D20B647A3}" name="Test Suite ID" dataDxfId="13" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{ED5D7682-7E0B-4088-9CEB-04199327A651}" name="Test Suite Name" dataDxfId="12" dataCellStyle="Normal">
+    <tableColumn id="1" xr3:uid="{27574F06-5BA9-4E63-97C7-825783688D46}" name="Test Case ID" dataDxfId="13" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{B526EB36-9DB5-49C2-8DA1-334D20B647A3}" name="Test Suite ID" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{ED5D7682-7E0B-4088-9CEB-04199327A651}" name="Test Suite Name" dataDxfId="11" dataCellStyle="Normal">
       <calculatedColumnFormula>_xlfn.XLOOKUP(tbl_TestCases[[#This Row],[Test Suite ID]],tbl_TestSuites[Test Suite ID],tbl_TestSuites[Test Suite Name], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{264D8F34-B394-4503-BE76-AED9935ABFB6}" name="Brief description" dataDxfId="11" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{FF5D68C7-F0C5-43FD-B3C6-0FD89A4C0BF0}" name="Expectation" dataDxfId="10" dataCellStyle="Normal"/>
-    <tableColumn id="6" xr3:uid="{AC820220-D268-4E52-AA4D-B6EB4A405E79}" name="Related steps (Count)" dataDxfId="9" dataCellStyle="Normal">
+    <tableColumn id="4" xr3:uid="{264D8F34-B394-4503-BE76-AED9935ABFB6}" name="Brief description" dataDxfId="10" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{FF5D68C7-F0C5-43FD-B3C6-0FD89A4C0BF0}" name="Expectation" dataDxfId="9" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{AC820220-D268-4E52-AA4D-B6EB4A405E79}" name="Related steps (Count)" dataDxfId="8" dataCellStyle="Normal">
       <calculatedColumnFormula>COUNTIF(tbl_Steps[Test Case ID], tbl_TestCases[[#This Row],[Test Case ID]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B73A8C2C-FDED-498D-9AE0-78ACB38485F6}" name="Steps passing (Count)" dataDxfId="8" dataCellStyle="Normal">
+    <tableColumn id="7" xr3:uid="{B73A8C2C-FDED-498D-9AE0-78ACB38485F6}" name="Steps passing (Count)" dataDxfId="7" dataCellStyle="Normal">
       <calculatedColumnFormula>COUNTIFS(tbl_Steps[Test Case ID],tbl_TestCases[[#This Row],[Test Case ID]],tbl_Steps[Grade], "PASS")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{4955DF23-818F-4B58-9ECE-732AC5472191}" name="Steps failing (Count)" dataDxfId="7" dataCellStyle="Normal">
+    <tableColumn id="8" xr3:uid="{4955DF23-818F-4B58-9ECE-732AC5472191}" name="Steps failing (Count)" dataDxfId="6" dataCellStyle="Normal">
       <calculatedColumnFormula>COUNTIFS(tbl_Steps[Test Case ID],tbl_TestCases[[#This Row],[Test Case ID]],tbl_Steps[Grade], "FAIL")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B8A6487D-B1AD-4036-A6F9-8446B575FA71}" name="Steps without grades (Count)" dataDxfId="6" dataCellStyle="Normal">
+    <tableColumn id="9" xr3:uid="{B8A6487D-B1AD-4036-A6F9-8446B575FA71}" name="Steps without grades (Count)" dataDxfId="5" dataCellStyle="Normal">
       <calculatedColumnFormula>tbl_TestCases[[#This Row],[Related steps (Count)]]-(tbl_TestCases[[#This Row],[Steps passing (Count)]]+tbl_TestCases[[#This Row],[Steps failing (Count)]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{AED18D94-50D3-4BF4-A6A3-650067C35BCE}" name="Grade from steps (%)" dataDxfId="5" dataCellStyle="Normal">
+    <tableColumn id="10" xr3:uid="{AED18D94-50D3-4BF4-A6A3-650067C35BCE}" name="Grade from steps (%)" dataDxfId="4" dataCellStyle="Normal">
       <calculatedColumnFormula>IFERROR(tbl_TestCases[[#This Row],[Steps passing (Count)]]/tbl_TestCases[[#This Row],[Related steps (Count)]],"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{710606B9-4D57-4EFC-A361-E7DB90F278AF}" name="Test Case Outcome" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{250EFB62-2850-48CE-AB17-75B4E454A4E2}" name="Test Case Grade" dataDxfId="3" dataCellStyle="Normal"/>
-    <tableColumn id="13" xr3:uid="{B6ECD6C7-48A9-4711-BB31-B5F8F17049F7}" name="Notes" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{710606B9-4D57-4EFC-A361-E7DB90F278AF}" name="Test Case Outcome" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{250EFB62-2850-48CE-AB17-75B4E454A4E2}" name="Test Case Grade" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{B6ECD6C7-48A9-4711-BB31-B5F8F17049F7}" name="Notes" dataDxfId="1" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1429,7 +1428,7 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B1" s="5">
         <f ca="1">NOW()</f>
-        <v>45636.761668634259</v>
+        <v>45636.778450347221</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.45">
@@ -1706,7 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F5C402-97F3-45C7-87D5-D390AFC3D58D}">
   <dimension ref="A17:M40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2688,8 +2687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE27539A-71A8-46AA-AE48-2B75AF98E22A}">
   <dimension ref="A17:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2727,46 +2726,44 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
         <v>4</v>
       </c>
-      <c r="C18" s="10" t="str">
+      <c r="C18" t="str">
         <f>_xlfn.XLOOKUP(tbl_Steps[[#This Row],[Test Case ID]],tbl_TestCases[Test Case ID],tbl_TestCases[Brief description], "")</f>
         <v>Pit data, Use default values</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18">
         <v>1</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
         <v>4</v>
       </c>
-      <c r="C19" s="10" t="str">
+      <c r="C19" t="str">
         <f>_xlfn.XLOOKUP(tbl_Steps[[#This Row],[Test Case ID]],tbl_TestCases[Test Case ID],tbl_TestCases[Brief description], "")</f>
         <v>Pit data, Use default values</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19">
         <v>2</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B20">
         <v>4</v>
@@ -2775,7 +2772,7 @@
         <f>_xlfn.XLOOKUP(tbl_Steps[[#This Row],[Test Case ID]],tbl_TestCases[Test Case ID],tbl_TestCases[Brief description], "")</f>
         <v>Pit data, Use default values</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20">
         <v>3</v>
       </c>
       <c r="E20" t="s">
@@ -2783,6 +2780,9 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>4</v>
+      </c>
       <c r="B21">
         <v>4</v>
       </c>
@@ -2790,7 +2790,7 @@
         <f>_xlfn.XLOOKUP(tbl_Steps[[#This Row],[Test Case ID]],tbl_TestCases[Test Case ID],tbl_TestCases[Brief description], "")</f>
         <v>Pit data, Use default values</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21">
         <v>4</v>
       </c>
       <c r="E21" t="s">
@@ -2798,44 +2798,43 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
         <v>4</v>
       </c>
-      <c r="C22" s="10" t="str">
+      <c r="C22" t="str">
         <f>_xlfn.XLOOKUP(tbl_Steps[[#This Row],[Test Case ID]],tbl_TestCases[Test Case ID],tbl_TestCases[Brief description], "")</f>
         <v>Pit data, Use default values</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22">
         <v>5</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" t="s">
         <v>65</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
         <v>4</v>
       </c>
-      <c r="C23" s="10" t="str">
+      <c r="C23" t="str">
         <f>_xlfn.XLOOKUP(tbl_Steps[[#This Row],[Test Case ID]],tbl_TestCases[Test Case ID],tbl_TestCases[Brief description], "")</f>
         <v>Pit data, Use default values</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23">
         <v>6</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more changes to teting manager
</commit_message>
<xml_diff>
--- a/Testing Manager.xlsx
+++ b/Testing Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\2024-10-ATAA-Forge\scouting-xtreme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338D0104-E534-460B-AB7F-A2539226F104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE338BBA-9375-499A-980C-48217DEC55A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12877" yWindow="0" windowWidth="13125" windowHeight="15563" activeTab="2" xr2:uid="{02701ECD-E265-41D5-A2A7-3CC6CA32D865}"/>
   </bookViews>
@@ -1428,7 +1428,7 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B1" s="5">
         <f ca="1">NOW()</f>
-        <v>45636.778450347221</v>
+        <v>45636.79013587963</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.45">
@@ -1705,7 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F5C402-97F3-45C7-87D5-D390AFC3D58D}">
   <dimension ref="A17:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -2687,7 +2687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE27539A-71A8-46AA-AE48-2B75AF98E22A}">
   <dimension ref="A17:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>

</xml_diff>